<commit_message>
got simple import done
</commit_message>
<xml_diff>
--- a/app/src/test/resources/de/ks/idnadrev/expimp/xls/thoughts.xlsx
+++ b/app/src/test/resources/de/ks/idnadrev/expimp/xls/thoughts.xlsx
@@ -474,6 +474,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -572,8 +573,8 @@
   </sheetPr>
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A115" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A144" activeCellId="0" pane="topLeft" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1734,7 +1735,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="143">
       <c r="A143" s="2" t="n">
-        <v>41887.8115128472</v>
+        <v>41887.8115277778</v>
       </c>
       <c r="C143" s="0" t="s">
         <v>147</v>

</xml_diff>